<commit_message>
Fix filter dimensions typo in excel sheets
</commit_message>
<xml_diff>
--- a/DeepBenchKernels_inference.xlsx
+++ b/DeepBenchKernels_inference.xlsx
@@ -135,12 +135,6 @@
     <t>K  (number of filters)</t>
   </si>
   <si>
-    <t>R (filter width)</t>
-  </si>
-  <si>
-    <t>S (filter height)</t>
-  </si>
-  <si>
     <t>KWS</t>
   </si>
   <si>
@@ -193,6 +187,12 @@
   </si>
   <si>
     <t>Deep Speech</t>
+  </si>
+  <si>
+    <t>R (filter height)</t>
+  </si>
+  <si>
+    <t>S (filter width)</t>
   </si>
 </sst>
 </file>
@@ -1197,8 +1197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q311"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A205" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1237,7 +1237,7 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I1" t="s">
         <v>7</v>
@@ -1263,7 +1263,7 @@
         <v>3</v>
       </c>
       <c r="H2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1286,7 +1286,7 @@
         <v>3</v>
       </c>
       <c r="H3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1309,7 +1309,7 @@
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1332,7 +1332,7 @@
         <v>3</v>
       </c>
       <c r="H5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1355,7 +1355,7 @@
         <v>3</v>
       </c>
       <c r="H6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1378,7 +1378,7 @@
         <v>3</v>
       </c>
       <c r="H7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1401,7 +1401,7 @@
         <v>3</v>
       </c>
       <c r="H8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1424,7 +1424,7 @@
         <v>3</v>
       </c>
       <c r="H9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1447,7 +1447,7 @@
         <v>3</v>
       </c>
       <c r="H10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1470,7 +1470,7 @@
         <v>3</v>
       </c>
       <c r="H11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1493,7 +1493,7 @@
         <v>3</v>
       </c>
       <c r="H12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1517,7 +1517,7 @@
         <v>3</v>
       </c>
       <c r="H13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1541,7 +1541,7 @@
         <v>3</v>
       </c>
       <c r="H14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1565,12 +1565,12 @@
         <v>3</v>
       </c>
       <c r="H15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="B16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C16">
         <v>64</v>
@@ -1588,7 +1588,7 @@
         <v>3</v>
       </c>
       <c r="H16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1611,7 +1611,7 @@
         <v>3</v>
       </c>
       <c r="H17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1634,7 +1634,7 @@
         <v>3</v>
       </c>
       <c r="H18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1657,7 +1657,7 @@
         <v>3</v>
       </c>
       <c r="H19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1680,7 +1680,7 @@
         <v>3</v>
       </c>
       <c r="H20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1703,7 +1703,7 @@
         <v>3</v>
       </c>
       <c r="H21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1726,12 +1726,12 @@
         <v>3</v>
       </c>
       <c r="H22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="B23" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C23">
         <v>1024</v>
@@ -1749,12 +1749,12 @@
         <v>3</v>
       </c>
       <c r="H23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="B24" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C24">
         <v>7680</v>
@@ -1772,13 +1772,13 @@
         <v>3</v>
       </c>
       <c r="H24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J24" s="2"/>
     </row>
     <row r="25" spans="1:10">
       <c r="B25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C25">
         <v>6144</v>
@@ -1796,14 +1796,14 @@
         <v>3</v>
       </c>
       <c r="H25" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J25" s="2"/>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C26" s="1">
         <v>4608</v>
@@ -1821,7 +1821,7 @@
         <v>3</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I26" s="1"/>
       <c r="J26" s="2"/>
@@ -1829,7 +1829,7 @@
     <row r="27" spans="1:10">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C27" s="1">
         <v>8448</v>
@@ -1847,7 +1847,7 @@
         <v>3</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I27" s="1"/>
       <c r="J27" s="2"/>
@@ -1855,7 +1855,7 @@
     <row r="28" spans="1:10">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C28" s="1">
         <v>3072</v>
@@ -1873,14 +1873,14 @@
         <v>3</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I28" s="1"/>
       <c r="J28" s="2"/>
     </row>
     <row r="29" spans="1:10">
       <c r="B29" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C29">
         <v>7680</v>
@@ -1898,13 +1898,13 @@
         <v>3</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J29" s="2"/>
     </row>
     <row r="30" spans="1:10">
       <c r="B30" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C30">
         <v>6144</v>
@@ -1922,14 +1922,14 @@
         <v>3</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J30" s="2"/>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C31" s="1">
         <v>4608</v>
@@ -1947,7 +1947,7 @@
         <v>3</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I31" s="1"/>
       <c r="J31" s="2"/>
@@ -1955,7 +1955,7 @@
     <row r="32" spans="1:10">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C32" s="1">
         <v>8448</v>
@@ -1973,7 +1973,7 @@
         <v>3</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I32" s="1"/>
       <c r="J32" s="2"/>
@@ -1981,7 +1981,7 @@
     <row r="33" spans="1:11">
       <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C33" s="1">
         <v>3072</v>
@@ -1999,14 +1999,14 @@
         <v>3</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I33" s="1"/>
       <c r="J33" s="2"/>
     </row>
     <row r="34" spans="1:11">
       <c r="B34" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C34">
         <v>7680</v>
@@ -2024,13 +2024,13 @@
         <v>3</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J34" s="2"/>
     </row>
     <row r="35" spans="1:11">
       <c r="B35" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C35">
         <v>6144</v>
@@ -2048,14 +2048,14 @@
         <v>3</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J35" s="2"/>
     </row>
     <row r="36" spans="1:11">
       <c r="A36" s="1"/>
       <c r="B36" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C36" s="1">
         <v>4608</v>
@@ -2073,7 +2073,7 @@
         <v>3</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I36" s="1"/>
       <c r="J36" s="2"/>
@@ -2081,7 +2081,7 @@
     <row r="37" spans="1:11">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C37" s="1">
         <v>8448</v>
@@ -2099,7 +2099,7 @@
         <v>3</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I37" s="1"/>
       <c r="J37" s="2"/>
@@ -2107,7 +2107,7 @@
     <row r="38" spans="1:11">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C38" s="1">
         <v>3072</v>
@@ -2125,7 +2125,7 @@
         <v>3</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I38" s="1"/>
       <c r="J38" s="2"/>
@@ -2133,7 +2133,7 @@
     <row r="39" spans="1:11">
       <c r="A39" s="1"/>
       <c r="B39" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C39" s="1">
         <v>6144</v>
@@ -2151,7 +2151,7 @@
         <v>3</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I39" s="1"/>
       <c r="J39" s="2"/>
@@ -2159,7 +2159,7 @@
     <row r="40" spans="1:11">
       <c r="A40" s="1"/>
       <c r="B40" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C40" s="1">
         <v>4608</v>
@@ -2177,7 +2177,7 @@
         <v>3</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I40" s="1"/>
       <c r="J40" s="2"/>
@@ -2185,7 +2185,7 @@
     <row r="41" spans="1:11">
       <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C41" s="1">
         <v>8448</v>
@@ -2203,7 +2203,7 @@
         <v>3</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I41" s="1"/>
       <c r="J41" s="2"/>
@@ -2211,7 +2211,7 @@
     <row r="42" spans="1:11">
       <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C42" s="1">
         <v>6144</v>
@@ -2229,7 +2229,7 @@
         <v>3</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I42" s="1"/>
       <c r="J42" s="2"/>
@@ -2237,7 +2237,7 @@
     <row r="43" spans="1:11">
       <c r="A43" s="1"/>
       <c r="B43" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C43" s="1">
         <v>4608</v>
@@ -2255,7 +2255,7 @@
         <v>3</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I43" s="1"/>
       <c r="J43" s="2"/>
@@ -2263,7 +2263,7 @@
     <row r="44" spans="1:11">
       <c r="A44" s="1"/>
       <c r="B44" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C44" s="1">
         <v>8448</v>
@@ -2281,7 +2281,7 @@
         <v>3</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I44" s="1"/>
       <c r="J44" s="2"/>
@@ -2289,7 +2289,7 @@
     <row r="45" spans="1:11">
       <c r="A45" s="1"/>
       <c r="B45" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C45" s="1">
         <v>6144</v>
@@ -2307,7 +2307,7 @@
         <v>3</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I45" s="1"/>
       <c r="J45" s="2"/>
@@ -2315,7 +2315,7 @@
     <row r="46" spans="1:11">
       <c r="A46" s="1"/>
       <c r="B46" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C46" s="1">
         <v>4608</v>
@@ -2333,7 +2333,7 @@
         <v>3</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I46" s="1"/>
       <c r="J46" s="2"/>
@@ -2341,7 +2341,7 @@
     <row r="47" spans="1:11">
       <c r="A47" s="1"/>
       <c r="B47" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C47" s="1">
         <v>8448</v>
@@ -2359,7 +2359,7 @@
         <v>3</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I47" s="1"/>
       <c r="J47" s="2"/>
@@ -2367,7 +2367,7 @@
     <row r="48" spans="1:11">
       <c r="A48" s="1"/>
       <c r="B48" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C48" s="1">
         <v>128</v>
@@ -2385,7 +2385,7 @@
         <v>3</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I48" s="1"/>
       <c r="J48" s="2"/>
@@ -2394,7 +2394,7 @@
     <row r="49" spans="1:11">
       <c r="A49" s="1"/>
       <c r="B49" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C49" s="1">
         <v>3072</v>
@@ -2412,7 +2412,7 @@
         <v>3</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I49" s="1"/>
       <c r="J49" s="2"/>
@@ -2421,7 +2421,7 @@
     <row r="50" spans="1:11">
       <c r="A50" s="1"/>
       <c r="B50" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C50" s="1">
         <v>128</v>
@@ -2439,7 +2439,7 @@
         <v>3</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I50" s="1"/>
       <c r="J50" s="2"/>
@@ -2448,7 +2448,7 @@
     <row r="51" spans="1:11">
       <c r="A51" s="1"/>
       <c r="B51" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C51" s="1">
         <v>3072</v>
@@ -2466,7 +2466,7 @@
         <v>3</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I51" s="1"/>
       <c r="J51" s="2"/>
@@ -2475,7 +2475,7 @@
     <row r="52" spans="1:11">
       <c r="A52" s="1"/>
       <c r="B52" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C52" s="1">
         <v>176</v>
@@ -2493,7 +2493,7 @@
         <v>3</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I52" s="1"/>
       <c r="J52" s="2"/>
@@ -2502,7 +2502,7 @@
     <row r="53" spans="1:11">
       <c r="A53" s="1"/>
       <c r="B53" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C53" s="1">
         <v>4224</v>
@@ -2520,7 +2520,7 @@
         <v>3</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I53" s="1"/>
       <c r="J53" s="2"/>
@@ -2529,7 +2529,7 @@
     <row r="54" spans="1:11">
       <c r="A54" s="1"/>
       <c r="B54" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C54" s="1">
         <v>128</v>
@@ -2547,7 +2547,7 @@
         <v>3</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I54" s="1"/>
       <c r="J54" s="2"/>
@@ -2556,7 +2556,7 @@
     <row r="55" spans="1:11">
       <c r="A55" s="1"/>
       <c r="B55" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C55" s="1">
         <v>4224</v>
@@ -2574,7 +2574,7 @@
         <v>3</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I55" s="1"/>
       <c r="J55" s="2"/>
@@ -2601,7 +2601,7 @@
         <v>3</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="57" spans="1:11">
@@ -2625,7 +2625,7 @@
         <v>3</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="58" spans="1:11">
@@ -2649,7 +2649,7 @@
         <v>3</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="59" spans="1:11">
@@ -2673,7 +2673,7 @@
         <v>3</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="60" spans="1:11">
@@ -2697,7 +2697,7 @@
         <v>3</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="61" spans="1:11">
@@ -2721,7 +2721,7 @@
         <v>3</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="62" spans="1:11">
@@ -2745,7 +2745,7 @@
         <v>3</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="63" spans="1:11">
@@ -2769,7 +2769,7 @@
         <v>3</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="64" spans="1:11">
@@ -2792,7 +2792,7 @@
         <v>3</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="65" spans="2:8">
@@ -2815,7 +2815,7 @@
         <v>3</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="66" spans="2:8">
@@ -2839,7 +2839,7 @@
         <v>3</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="67" spans="2:8">
@@ -2863,7 +2863,7 @@
         <v>3</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="68" spans="2:8">
@@ -2887,7 +2887,7 @@
         <v>3</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="69" spans="2:8">
@@ -2911,7 +2911,7 @@
         <v>3</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="70" spans="2:8">
@@ -2935,7 +2935,7 @@
         <v>3</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="71" spans="2:8">
@@ -2959,7 +2959,7 @@
         <v>3</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="72" spans="2:8">
@@ -2983,7 +2983,7 @@
         <v>3</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="73" spans="2:8">
@@ -3007,7 +3007,7 @@
         <v>3</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="74" spans="2:8">
@@ -3030,7 +3030,7 @@
         <v>3</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="75" spans="2:8">
@@ -3053,7 +3053,7 @@
         <v>3</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="76" spans="2:8">
@@ -3077,7 +3077,7 @@
         <v>3</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="77" spans="2:8">
@@ -3101,7 +3101,7 @@
         <v>3</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="78" spans="2:8">
@@ -3125,7 +3125,7 @@
         <v>3</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="79" spans="2:8">
@@ -3149,7 +3149,7 @@
         <v>3</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="80" spans="2:8">
@@ -3173,7 +3173,7 @@
         <v>3</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="81" spans="1:10">
@@ -3197,7 +3197,7 @@
         <v>3</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="82" spans="1:10">
@@ -3221,7 +3221,7 @@
         <v>3</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="83" spans="1:10">
@@ -3245,7 +3245,7 @@
         <v>3</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="84" spans="1:10">
@@ -3268,7 +3268,7 @@
         <v>3</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="85" spans="1:10">
@@ -3291,7 +3291,7 @@
         <v>3</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="86" spans="1:10">
@@ -3332,7 +3332,7 @@
     </row>
     <row r="89" spans="1:10">
       <c r="A89" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B89" t="s">
         <v>24</v>
@@ -3353,10 +3353,10 @@
         <v>6</v>
       </c>
       <c r="H89" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I89" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J89" t="s">
         <v>7</v>
@@ -3385,7 +3385,7 @@
         <v>0.95</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="91" spans="1:10">
@@ -3411,7 +3411,7 @@
         <v>0.95</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="92" spans="1:10">
@@ -3437,7 +3437,7 @@
         <v>0.95</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="93" spans="1:10">
@@ -3463,7 +3463,7 @@
         <v>0.95</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="94" spans="1:10">
@@ -3489,7 +3489,7 @@
         <v>0.95</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="95" spans="1:10">
@@ -3515,7 +3515,7 @@
         <v>0.95</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="96" spans="1:10">
@@ -3541,7 +3541,7 @@
         <v>0.95</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="97" spans="2:9">
@@ -3567,7 +3567,7 @@
         <v>0.95</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="98" spans="2:9">
@@ -3593,7 +3593,7 @@
         <v>0.95</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="99" spans="2:9">
@@ -3619,7 +3619,7 @@
         <v>0.95</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="100" spans="2:9">
@@ -3645,7 +3645,7 @@
         <v>0.95</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="101" spans="2:9">
@@ -3671,7 +3671,7 @@
         <v>0.95</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="102" spans="2:9">
@@ -3697,7 +3697,7 @@
         <v>0.9</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="103" spans="2:9">
@@ -3723,7 +3723,7 @@
         <v>0.9</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="104" spans="2:9">
@@ -3749,7 +3749,7 @@
         <v>0.9</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="105" spans="2:9">
@@ -3775,7 +3775,7 @@
         <v>0.9</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="106" spans="2:9">
@@ -3801,7 +3801,7 @@
         <v>0.9</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="107" spans="2:9">
@@ -3827,7 +3827,7 @@
         <v>0.9</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="108" spans="2:9">
@@ -3853,7 +3853,7 @@
         <v>0.9</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="109" spans="2:9">
@@ -3879,7 +3879,7 @@
         <v>0.9</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="110" spans="2:9">
@@ -3905,7 +3905,7 @@
         <v>0.9</v>
       </c>
       <c r="I110" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="111" spans="2:9">
@@ -3931,7 +3931,7 @@
         <v>0.9</v>
       </c>
       <c r="I111" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="112" spans="2:9">
@@ -3957,7 +3957,7 @@
         <v>0.9</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="113" spans="1:17">
@@ -3983,7 +3983,7 @@
         <v>0.9</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="114" spans="1:17">
@@ -4026,10 +4026,10 @@
         <v>36</v>
       </c>
       <c r="H117" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="I117" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="J117" t="s">
         <v>20</v>
@@ -4044,7 +4044,7 @@
         <v>23</v>
       </c>
       <c r="N117" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="O117" t="s">
         <v>13</v>
@@ -4094,7 +4094,7 @@
         <v>2</v>
       </c>
       <c r="N118" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="119" spans="1:17">
@@ -4135,7 +4135,7 @@
         <v>2</v>
       </c>
       <c r="N119" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="120" spans="1:17">
@@ -4176,7 +4176,7 @@
         <v>2</v>
       </c>
       <c r="N120" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="121" spans="1:17">
@@ -4217,7 +4217,7 @@
         <v>2</v>
       </c>
       <c r="N121" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="122" spans="1:17">
@@ -4258,7 +4258,7 @@
         <v>2</v>
       </c>
       <c r="N122" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="123" spans="1:17">
@@ -4299,7 +4299,7 @@
         <v>2</v>
       </c>
       <c r="N123" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="124" spans="1:17">
@@ -4340,7 +4340,7 @@
         <v>1</v>
       </c>
       <c r="N124" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="125" spans="1:17">
@@ -4381,7 +4381,7 @@
         <v>1</v>
       </c>
       <c r="N125" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="126" spans="1:17">
@@ -4422,7 +4422,7 @@
         <v>1</v>
       </c>
       <c r="N126" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="127" spans="1:17">
@@ -4463,7 +4463,7 @@
         <v>1</v>
       </c>
       <c r="N127" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="128" spans="1:17">
@@ -4504,7 +4504,7 @@
         <v>2</v>
       </c>
       <c r="N128" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="129" spans="2:14">
@@ -4545,7 +4545,7 @@
         <v>1</v>
       </c>
       <c r="N129" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="130" spans="2:14">
@@ -4586,7 +4586,7 @@
         <v>1</v>
       </c>
       <c r="N130" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="131" spans="2:14">
@@ -4627,7 +4627,7 @@
         <v>1</v>
       </c>
       <c r="N131" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="132" spans="2:14">
@@ -4668,7 +4668,7 @@
         <v>1</v>
       </c>
       <c r="N132" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="133" spans="2:14">
@@ -4709,7 +4709,7 @@
         <v>1</v>
       </c>
       <c r="N133" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="134" spans="2:14">
@@ -4750,7 +4750,7 @@
         <v>1</v>
       </c>
       <c r="N134" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="135" spans="2:14">
@@ -4792,7 +4792,7 @@
         <v>1</v>
       </c>
       <c r="N135" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="136" spans="2:14">
@@ -4834,7 +4834,7 @@
         <v>1</v>
       </c>
       <c r="N136" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="137" spans="2:14">
@@ -4875,7 +4875,7 @@
         <v>1</v>
       </c>
       <c r="N137" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="138" spans="2:14">
@@ -4916,7 +4916,7 @@
         <v>1</v>
       </c>
       <c r="N138" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="139" spans="2:14">
@@ -4957,7 +4957,7 @@
         <v>1</v>
       </c>
       <c r="N139" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="140" spans="2:14">
@@ -4998,7 +4998,7 @@
         <v>1</v>
       </c>
       <c r="N140" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="141" spans="2:14">
@@ -5040,7 +5040,7 @@
         <v>1</v>
       </c>
       <c r="N141" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="142" spans="2:14">
@@ -5082,7 +5082,7 @@
         <v>1</v>
       </c>
       <c r="N142" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="143" spans="2:14">
@@ -5123,7 +5123,7 @@
         <v>1</v>
       </c>
       <c r="N143" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="144" spans="2:14">
@@ -5164,7 +5164,7 @@
         <v>1</v>
       </c>
       <c r="N144" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="145" spans="2:14">
@@ -5205,7 +5205,7 @@
         <v>2</v>
       </c>
       <c r="N145" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="146" spans="2:14">
@@ -5246,7 +5246,7 @@
         <v>1</v>
       </c>
       <c r="N146" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="147" spans="2:14">
@@ -5287,7 +5287,7 @@
         <v>1</v>
       </c>
       <c r="N147" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="148" spans="2:14">
@@ -5328,7 +5328,7 @@
         <v>1</v>
       </c>
       <c r="N148" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="149" spans="2:14">
@@ -5369,7 +5369,7 @@
         <v>1</v>
       </c>
       <c r="N149" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="150" spans="2:14">
@@ -5410,7 +5410,7 @@
         <v>1</v>
       </c>
       <c r="N150" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="151" spans="2:14">
@@ -5451,7 +5451,7 @@
         <v>1</v>
       </c>
       <c r="N151" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="152" spans="2:14">
@@ -5492,7 +5492,7 @@
         <v>2</v>
       </c>
       <c r="N152" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="153" spans="2:14">
@@ -5533,7 +5533,7 @@
         <v>1</v>
       </c>
       <c r="N153" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="154" spans="2:14">
@@ -5574,7 +5574,7 @@
         <v>1</v>
       </c>
       <c r="N154" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="155" spans="2:14">
@@ -5615,7 +5615,7 @@
         <v>1</v>
       </c>
       <c r="N155" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="156" spans="2:14">
@@ -5656,7 +5656,7 @@
         <v>1</v>
       </c>
       <c r="N156" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="157" spans="2:14">
@@ -5697,7 +5697,7 @@
         <v>1</v>
       </c>
       <c r="N157" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="158" spans="2:14">
@@ -5738,12 +5738,12 @@
         <v>1</v>
       </c>
       <c r="N158" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="159" spans="2:14">
       <c r="B159" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C159">
         <v>151</v>
@@ -5779,12 +5779,12 @@
         <v>8</v>
       </c>
       <c r="N159" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="160" spans="2:14">
       <c r="B160" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C160">
         <v>56</v>
@@ -5820,12 +5820,12 @@
         <v>1</v>
       </c>
       <c r="N160" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="161" spans="2:14">
       <c r="B161" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C161">
         <v>56</v>
@@ -5861,12 +5861,12 @@
         <v>2</v>
       </c>
       <c r="N161" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="162" spans="2:14">
       <c r="B162" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C162">
         <v>28</v>
@@ -5902,12 +5902,12 @@
         <v>1</v>
       </c>
       <c r="N162" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="163" spans="2:14">
       <c r="B163" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C163" s="1">
         <v>28</v>
@@ -5943,12 +5943,12 @@
         <v>2</v>
       </c>
       <c r="N163" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="164" spans="2:14">
       <c r="B164" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C164">
         <v>14</v>
@@ -5984,12 +5984,12 @@
         <v>1</v>
       </c>
       <c r="N164" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="165" spans="2:14">
       <c r="B165" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C165">
         <v>14</v>
@@ -6025,12 +6025,12 @@
         <v>1</v>
       </c>
       <c r="N165" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="166" spans="2:14">
       <c r="B166" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C166" s="1">
         <v>14</v>
@@ -6066,12 +6066,12 @@
         <v>2</v>
       </c>
       <c r="N166" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="167" spans="2:14">
       <c r="B167" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C167">
         <v>7</v>
@@ -6107,12 +6107,12 @@
         <v>1</v>
       </c>
       <c r="N167" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="168" spans="2:14">
       <c r="B168" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C168">
         <v>7</v>
@@ -6148,12 +6148,12 @@
         <v>2</v>
       </c>
       <c r="N168" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="169" spans="2:14">
       <c r="B169" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C169">
         <v>56</v>
@@ -6189,12 +6189,12 @@
         <v>1</v>
       </c>
       <c r="N169" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="170" spans="2:14">
       <c r="B170" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C170">
         <v>56</v>
@@ -6230,12 +6230,12 @@
         <v>2</v>
       </c>
       <c r="N170" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="171" spans="2:14">
       <c r="B171" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C171">
         <v>28</v>
@@ -6271,12 +6271,12 @@
         <v>1</v>
       </c>
       <c r="N171" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="172" spans="2:14">
       <c r="B172" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C172" s="1">
         <v>28</v>
@@ -6312,12 +6312,12 @@
         <v>2</v>
       </c>
       <c r="N172" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="173" spans="2:14">
       <c r="B173" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C173">
         <v>14</v>
@@ -6353,12 +6353,12 @@
         <v>1</v>
       </c>
       <c r="N173" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="174" spans="2:14">
       <c r="B174" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C174">
         <v>14</v>
@@ -6394,12 +6394,12 @@
         <v>1</v>
       </c>
       <c r="N174" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="175" spans="2:14">
       <c r="B175" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C175" s="1">
         <v>14</v>
@@ -6435,12 +6435,12 @@
         <v>2</v>
       </c>
       <c r="N175" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="176" spans="2:14">
       <c r="B176" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C176">
         <v>7</v>
@@ -6476,12 +6476,12 @@
         <v>1</v>
       </c>
       <c r="N176" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="177" spans="2:14">
       <c r="B177" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C177">
         <v>7</v>
@@ -6517,12 +6517,12 @@
         <v>2</v>
       </c>
       <c r="N177" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="178" spans="2:14">
       <c r="B178" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C178">
         <v>700</v>
@@ -6558,12 +6558,12 @@
         <v>2</v>
       </c>
       <c r="N178" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="179" spans="2:14">
       <c r="B179" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C179">
         <v>350</v>
@@ -6599,12 +6599,12 @@
         <v>1</v>
       </c>
       <c r="N179" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="180" spans="2:14">
       <c r="B180" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C180">
         <v>350</v>
@@ -6640,12 +6640,12 @@
         <v>2</v>
       </c>
       <c r="N180" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="181" spans="2:14">
       <c r="B181" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C181">
         <v>175</v>
@@ -6681,12 +6681,12 @@
         <v>1</v>
       </c>
       <c r="N181" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="182" spans="2:14">
       <c r="B182" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C182">
         <v>175</v>
@@ -6722,12 +6722,12 @@
         <v>2</v>
       </c>
       <c r="N182" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="183" spans="2:14">
       <c r="B183" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C183">
         <v>84</v>
@@ -6763,12 +6763,12 @@
         <v>1</v>
       </c>
       <c r="N183" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="184" spans="2:14">
       <c r="B184" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C184">
         <v>84</v>
@@ -6804,12 +6804,12 @@
         <v>2</v>
       </c>
       <c r="N184" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="185" spans="2:14">
       <c r="B185" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C185">
         <v>42</v>
@@ -6845,12 +6845,12 @@
         <v>1</v>
       </c>
       <c r="N185" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="186" spans="2:14">
       <c r="B186" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C186">
         <v>700</v>
@@ -6886,12 +6886,12 @@
         <v>2</v>
       </c>
       <c r="N186" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="187" spans="2:14">
       <c r="B187" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C187">
         <v>350</v>
@@ -6927,12 +6927,12 @@
         <v>1</v>
       </c>
       <c r="N187" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="188" spans="2:14">
       <c r="B188" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C188">
         <v>350</v>
@@ -6968,12 +6968,12 @@
         <v>2</v>
       </c>
       <c r="N188" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="189" spans="2:14">
       <c r="B189" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C189">
         <v>175</v>
@@ -7009,12 +7009,12 @@
         <v>1</v>
       </c>
       <c r="N189" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="190" spans="2:14">
       <c r="B190" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C190">
         <v>175</v>
@@ -7050,12 +7050,12 @@
         <v>2</v>
       </c>
       <c r="N190" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="191" spans="2:14">
       <c r="B191" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C191">
         <v>84</v>
@@ -7091,12 +7091,12 @@
         <v>1</v>
       </c>
       <c r="N191" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="192" spans="2:14">
       <c r="B192" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C192">
         <v>84</v>
@@ -7132,12 +7132,12 @@
         <v>2</v>
       </c>
       <c r="N192" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="193" spans="1:14">
       <c r="B193" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C193">
         <v>42</v>
@@ -7173,13 +7173,13 @@
         <v>1</v>
       </c>
       <c r="N193" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="194" spans="1:14">
       <c r="A194" s="1"/>
       <c r="B194" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C194">
         <v>112</v>
@@ -7215,13 +7215,13 @@
         <v>1</v>
       </c>
       <c r="N194" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="195" spans="1:14">
       <c r="A195" s="1"/>
       <c r="B195" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C195">
         <v>56</v>
@@ -7257,13 +7257,13 @@
         <v>1</v>
       </c>
       <c r="N195" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="196" spans="1:14">
       <c r="A196" s="1"/>
       <c r="B196" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C196">
         <v>56</v>
@@ -7299,13 +7299,13 @@
         <v>1</v>
       </c>
       <c r="N196" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="197" spans="1:14">
       <c r="A197" s="1"/>
       <c r="B197" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C197">
         <v>56</v>
@@ -7341,13 +7341,13 @@
         <v>2</v>
       </c>
       <c r="N197" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="198" spans="1:14">
       <c r="A198" s="1"/>
       <c r="B198" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C198" s="1">
         <v>28</v>
@@ -7383,13 +7383,13 @@
         <v>1</v>
       </c>
       <c r="N198" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="199" spans="1:14">
       <c r="A199" s="1"/>
       <c r="B199" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C199" s="1">
         <v>28</v>
@@ -7425,13 +7425,13 @@
         <v>1</v>
       </c>
       <c r="N199" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="200" spans="1:14">
       <c r="A200" s="1"/>
       <c r="B200" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C200" s="1">
         <v>28</v>
@@ -7467,13 +7467,13 @@
         <v>2</v>
       </c>
       <c r="N200" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="201" spans="1:14">
       <c r="A201" s="1"/>
       <c r="B201" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C201" s="1">
         <v>14</v>
@@ -7509,13 +7509,13 @@
         <v>1</v>
       </c>
       <c r="N201" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="202" spans="1:14">
       <c r="A202" s="1"/>
       <c r="B202" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C202" s="1">
         <v>28</v>
@@ -7551,13 +7551,13 @@
         <v>2</v>
       </c>
       <c r="N202" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="203" spans="1:14">
       <c r="A203" s="1"/>
       <c r="B203" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C203" s="1">
         <v>14</v>
@@ -7593,13 +7593,13 @@
         <v>1</v>
       </c>
       <c r="N203" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="204" spans="1:14">
       <c r="A204" s="1"/>
       <c r="B204" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C204" s="1">
         <v>14</v>
@@ -7635,13 +7635,13 @@
         <v>1</v>
       </c>
       <c r="N204" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="205" spans="1:14">
       <c r="A205" s="1"/>
       <c r="B205" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C205" s="1">
         <v>14</v>
@@ -7677,13 +7677,13 @@
         <v>2</v>
       </c>
       <c r="N205" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="206" spans="1:14">
       <c r="A206" s="1"/>
       <c r="B206" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C206" s="1">
         <v>7</v>
@@ -7719,13 +7719,13 @@
         <v>1</v>
       </c>
       <c r="N206" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="207" spans="1:14">
       <c r="A207" s="1"/>
       <c r="B207" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C207" s="1">
         <v>7</v>
@@ -7761,13 +7761,13 @@
         <v>1</v>
       </c>
       <c r="N207" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="208" spans="1:14">
       <c r="A208" s="1"/>
       <c r="B208" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C208" s="1">
         <v>14</v>
@@ -7803,13 +7803,13 @@
         <v>2</v>
       </c>
       <c r="N208" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="209" spans="1:14">
       <c r="A209" s="1"/>
       <c r="B209" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C209" s="1">
         <v>7</v>
@@ -7845,13 +7845,13 @@
         <v>1</v>
       </c>
       <c r="N209" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="210" spans="1:14">
       <c r="A210" s="1"/>
       <c r="B210" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C210">
         <v>112</v>
@@ -7887,13 +7887,13 @@
         <v>1</v>
       </c>
       <c r="N210" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="211" spans="1:14">
       <c r="A211" s="1"/>
       <c r="B211" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C211">
         <v>56</v>
@@ -7929,13 +7929,13 @@
         <v>1</v>
       </c>
       <c r="N211" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="212" spans="1:14">
       <c r="A212" s="1"/>
       <c r="B212" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C212">
         <v>56</v>
@@ -7971,13 +7971,13 @@
         <v>1</v>
       </c>
       <c r="N212" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="213" spans="1:14">
       <c r="A213" s="1"/>
       <c r="B213" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C213">
         <v>56</v>
@@ -8013,13 +8013,13 @@
         <v>2</v>
       </c>
       <c r="N213" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="214" spans="1:14">
       <c r="A214" s="1"/>
       <c r="B214" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C214" s="1">
         <v>28</v>
@@ -8055,13 +8055,13 @@
         <v>1</v>
       </c>
       <c r="N214" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="215" spans="1:14">
       <c r="A215" s="1"/>
       <c r="B215" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C215" s="1">
         <v>28</v>
@@ -8097,13 +8097,13 @@
         <v>1</v>
       </c>
       <c r="N215" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="216" spans="1:14">
       <c r="A216" s="1"/>
       <c r="B216" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C216" s="1">
         <v>28</v>
@@ -8139,13 +8139,13 @@
         <v>2</v>
       </c>
       <c r="N216" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="217" spans="1:14">
       <c r="A217" s="1"/>
       <c r="B217" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C217" s="1">
         <v>14</v>
@@ -8181,13 +8181,13 @@
         <v>1</v>
       </c>
       <c r="N217" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="218" spans="1:14">
       <c r="A218" s="1"/>
       <c r="B218" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C218" s="1">
         <v>28</v>
@@ -8223,13 +8223,13 @@
         <v>2</v>
       </c>
       <c r="N218" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="219" spans="1:14">
       <c r="A219" s="1"/>
       <c r="B219" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C219" s="1">
         <v>14</v>
@@ -8265,13 +8265,13 @@
         <v>1</v>
       </c>
       <c r="N219" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="220" spans="1:14">
       <c r="A220" s="1"/>
       <c r="B220" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C220" s="1">
         <v>14</v>
@@ -8307,13 +8307,13 @@
         <v>1</v>
       </c>
       <c r="N220" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="221" spans="1:14">
       <c r="A221" s="1"/>
       <c r="B221" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C221" s="1">
         <v>14</v>
@@ -8349,13 +8349,13 @@
         <v>2</v>
       </c>
       <c r="N221" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="222" spans="1:14">
       <c r="A222" s="1"/>
       <c r="B222" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C222" s="1">
         <v>7</v>
@@ -8391,13 +8391,13 @@
         <v>1</v>
       </c>
       <c r="N222" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="223" spans="1:14">
       <c r="A223" s="1"/>
       <c r="B223" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C223" s="1">
         <v>7</v>
@@ -8433,13 +8433,13 @@
         <v>1</v>
       </c>
       <c r="N223" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="224" spans="1:14">
       <c r="A224" s="1"/>
       <c r="B224" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C224" s="1">
         <v>14</v>
@@ -8475,13 +8475,13 @@
         <v>2</v>
       </c>
       <c r="N224" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="225" spans="1:14">
       <c r="A225" s="1"/>
       <c r="B225" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C225" s="1">
         <v>7</v>
@@ -8517,7 +8517,7 @@
         <v>1</v>
       </c>
       <c r="N225" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="226" spans="1:14">
@@ -8556,7 +8556,7 @@
         <v>12</v>
       </c>
       <c r="F232" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G232" t="s">
         <v>16</v>
@@ -8567,7 +8567,7 @@
     </row>
     <row r="234" spans="1:14">
       <c r="B234" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C234" s="1">
         <v>32</v>
@@ -8579,12 +8579,12 @@
         <v>672</v>
       </c>
       <c r="F234" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="235" spans="1:14">
       <c r="B235" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C235" s="1">
         <v>32</v>
@@ -8596,7 +8596,7 @@
         <v>96</v>
       </c>
       <c r="F235" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="239" spans="1:14">
@@ -8616,7 +8616,7 @@
         <v>12</v>
       </c>
       <c r="F239" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G239" t="s">
         <v>18</v>
@@ -8639,7 +8639,7 @@
         <v>25</v>
       </c>
       <c r="F240" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="241" spans="2:6">
@@ -8656,7 +8656,7 @@
         <v>25</v>
       </c>
       <c r="F241" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="242" spans="2:6">
@@ -8673,7 +8673,7 @@
         <v>25</v>
       </c>
       <c r="F242" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="243" spans="2:6">
@@ -8690,7 +8690,7 @@
         <v>25</v>
       </c>
       <c r="F243" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="244" spans="2:6">
@@ -8707,7 +8707,7 @@
         <v>25</v>
       </c>
       <c r="F244" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="245" spans="2:6">
@@ -8724,7 +8724,7 @@
         <v>25</v>
       </c>
       <c r="F245" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="246" spans="2:6">
@@ -8741,7 +8741,7 @@
         <v>25</v>
       </c>
       <c r="F246" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="247" spans="2:6">
@@ -8758,7 +8758,7 @@
         <v>25</v>
       </c>
       <c r="F247" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="248" spans="2:6">
@@ -8775,7 +8775,7 @@
         <v>25</v>
       </c>
       <c r="F248" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="249" spans="2:6">
@@ -8792,7 +8792,7 @@
         <v>50</v>
       </c>
       <c r="F249" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="250" spans="2:6">
@@ -8809,7 +8809,7 @@
         <v>50</v>
       </c>
       <c r="F250" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="251" spans="2:6">
@@ -8826,12 +8826,12 @@
         <v>50</v>
       </c>
       <c r="F251" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="252" spans="2:6">
       <c r="B252" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C252">
         <v>256</v>
@@ -8843,12 +8843,12 @@
         <v>150</v>
       </c>
       <c r="F252" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="253" spans="2:6">
       <c r="B253" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C253">
         <v>256</v>
@@ -8860,12 +8860,12 @@
         <v>150</v>
       </c>
       <c r="F253" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="254" spans="2:6">
       <c r="B254" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C254">
         <v>256</v>
@@ -8877,18 +8877,18 @@
         <v>150</v>
       </c>
       <c r="F254" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="257" spans="1:8">
       <c r="A257" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B257" t="s">
         <v>24</v>
       </c>
       <c r="C257" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D257" t="s">
         <v>3</v>
@@ -8897,7 +8897,7 @@
         <v>12</v>
       </c>
       <c r="F257" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G257" t="s">
         <v>18</v>
@@ -8908,7 +8908,7 @@
     </row>
     <row r="258" spans="1:8">
       <c r="B258" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C258">
         <v>2816</v>
@@ -8920,12 +8920,12 @@
         <v>1500</v>
       </c>
       <c r="F258" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="259" spans="1:8">
       <c r="B259" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C259">
         <v>2816</v>
@@ -8937,12 +8937,12 @@
         <v>750</v>
       </c>
       <c r="F259" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="260" spans="1:8">
       <c r="B260" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C260">
         <v>2816</v>
@@ -8954,12 +8954,12 @@
         <v>375</v>
       </c>
       <c r="F260" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="261" spans="1:8">
       <c r="B261" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C261">
         <v>2816</v>
@@ -8971,12 +8971,12 @@
         <v>187</v>
       </c>
       <c r="F261" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="262" spans="1:8">
       <c r="B262" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C262">
         <v>2816</v>
@@ -8988,12 +8988,12 @@
         <v>1500</v>
       </c>
       <c r="F262" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="263" spans="1:8">
       <c r="B263" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C263">
         <v>2816</v>
@@ -9005,12 +9005,12 @@
         <v>750</v>
       </c>
       <c r="F263" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="264" spans="1:8">
       <c r="B264" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C264">
         <v>2816</v>
@@ -9022,12 +9022,12 @@
         <v>375</v>
       </c>
       <c r="F264" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="265" spans="1:8">
       <c r="B265" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C265">
         <v>2816</v>
@@ -9039,12 +9039,12 @@
         <v>187</v>
       </c>
       <c r="F265" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="266" spans="1:8">
       <c r="B266" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C266">
         <v>2816</v>
@@ -9056,12 +9056,12 @@
         <v>1500</v>
       </c>
       <c r="F266" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="267" spans="1:8">
       <c r="B267" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C267">
         <v>2816</v>
@@ -9073,12 +9073,12 @@
         <v>750</v>
       </c>
       <c r="F267" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="268" spans="1:8">
       <c r="B268" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C268">
         <v>2816</v>
@@ -9090,12 +9090,12 @@
         <v>375</v>
       </c>
       <c r="F268" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="269" spans="1:8">
       <c r="B269" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C269">
         <v>2816</v>
@@ -9107,12 +9107,12 @@
         <v>187</v>
       </c>
       <c r="F269" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="270" spans="1:8">
       <c r="B270" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C270">
         <v>2048</v>
@@ -9124,12 +9124,12 @@
         <v>1500</v>
       </c>
       <c r="F270" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="271" spans="1:8">
       <c r="B271" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C271">
         <v>2048</v>
@@ -9141,12 +9141,12 @@
         <v>750</v>
       </c>
       <c r="F271" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="272" spans="1:8">
       <c r="B272" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C272">
         <v>2048</v>
@@ -9158,12 +9158,12 @@
         <v>375</v>
       </c>
       <c r="F272" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="273" spans="2:6">
       <c r="B273" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C273">
         <v>2048</v>
@@ -9175,12 +9175,12 @@
         <v>187</v>
       </c>
       <c r="F273" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="274" spans="2:6">
       <c r="B274" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C274">
         <v>2048</v>
@@ -9192,12 +9192,12 @@
         <v>1500</v>
       </c>
       <c r="F274" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="275" spans="2:6">
       <c r="B275" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C275">
         <v>2048</v>
@@ -9209,12 +9209,12 @@
         <v>750</v>
       </c>
       <c r="F275" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="276" spans="2:6">
       <c r="B276" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C276">
         <v>2048</v>
@@ -9226,12 +9226,12 @@
         <v>375</v>
       </c>
       <c r="F276" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="277" spans="2:6">
       <c r="B277" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C277">
         <v>2048</v>
@@ -9243,12 +9243,12 @@
         <v>187</v>
       </c>
       <c r="F277" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="278" spans="2:6">
       <c r="B278" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C278">
         <v>2048</v>
@@ -9260,12 +9260,12 @@
         <v>1500</v>
       </c>
       <c r="F278" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="279" spans="2:6">
       <c r="B279" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C279">
         <v>2048</v>
@@ -9277,12 +9277,12 @@
         <v>750</v>
       </c>
       <c r="F279" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="280" spans="2:6">
       <c r="B280" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C280">
         <v>2048</v>
@@ -9294,12 +9294,12 @@
         <v>375</v>
       </c>
       <c r="F280" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="281" spans="2:6">
       <c r="B281" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C281">
         <v>2048</v>
@@ -9311,12 +9311,12 @@
         <v>187</v>
       </c>
       <c r="F281" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="282" spans="2:6">
       <c r="B282" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C282">
         <v>1536</v>
@@ -9328,12 +9328,12 @@
         <v>1500</v>
       </c>
       <c r="F282" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="283" spans="2:6">
       <c r="B283" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C283">
         <v>1536</v>
@@ -9345,12 +9345,12 @@
         <v>750</v>
       </c>
       <c r="F283" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="284" spans="2:6">
       <c r="B284" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C284">
         <v>1536</v>
@@ -9362,12 +9362,12 @@
         <v>375</v>
       </c>
       <c r="F284" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="285" spans="2:6">
       <c r="B285" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C285">
         <v>1536</v>
@@ -9379,12 +9379,12 @@
         <v>187</v>
       </c>
       <c r="F285" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="286" spans="2:6">
       <c r="B286" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C286">
         <v>1536</v>
@@ -9396,12 +9396,12 @@
         <v>1500</v>
       </c>
       <c r="F286" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="287" spans="2:6">
       <c r="B287" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C287">
         <v>1536</v>
@@ -9413,12 +9413,12 @@
         <v>750</v>
       </c>
       <c r="F287" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="288" spans="2:6">
       <c r="B288" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C288">
         <v>1536</v>
@@ -9430,12 +9430,12 @@
         <v>375</v>
       </c>
       <c r="F288" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="289" spans="2:6">
       <c r="B289" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C289">
         <v>1536</v>
@@ -9447,12 +9447,12 @@
         <v>187</v>
       </c>
       <c r="F289" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="290" spans="2:6">
       <c r="B290" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C290">
         <v>1536</v>
@@ -9464,12 +9464,12 @@
         <v>1500</v>
       </c>
       <c r="F290" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="291" spans="2:6">
       <c r="B291" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C291">
         <v>1536</v>
@@ -9481,12 +9481,12 @@
         <v>750</v>
       </c>
       <c r="F291" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="292" spans="2:6">
       <c r="B292" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C292">
         <v>1536</v>
@@ -9498,12 +9498,12 @@
         <v>375</v>
       </c>
       <c r="F292" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="293" spans="2:6">
       <c r="B293" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C293">
         <v>1536</v>
@@ -9515,12 +9515,12 @@
         <v>187</v>
       </c>
       <c r="F293" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="294" spans="2:6">
       <c r="B294" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C294">
         <v>2560</v>
@@ -9532,12 +9532,12 @@
         <v>1500</v>
       </c>
       <c r="F294" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="295" spans="2:6">
       <c r="B295" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C295">
         <v>2560</v>
@@ -9549,12 +9549,12 @@
         <v>750</v>
       </c>
       <c r="F295" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="296" spans="2:6">
       <c r="B296" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C296">
         <v>2560</v>
@@ -9566,12 +9566,12 @@
         <v>375</v>
       </c>
       <c r="F296" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="297" spans="2:6">
       <c r="B297" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C297">
         <v>2560</v>
@@ -9583,12 +9583,12 @@
         <v>187</v>
       </c>
       <c r="F297" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="298" spans="2:6">
       <c r="B298" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C298">
         <v>2560</v>
@@ -9600,12 +9600,12 @@
         <v>1500</v>
       </c>
       <c r="F298" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="299" spans="2:6">
       <c r="B299" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C299">
         <v>2560</v>
@@ -9617,12 +9617,12 @@
         <v>750</v>
       </c>
       <c r="F299" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="300" spans="2:6">
       <c r="B300" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C300">
         <v>2560</v>
@@ -9634,12 +9634,12 @@
         <v>375</v>
       </c>
       <c r="F300" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="301" spans="2:6">
       <c r="B301" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C301">
         <v>2560</v>
@@ -9651,12 +9651,12 @@
         <v>187</v>
       </c>
       <c r="F301" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="302" spans="2:6">
       <c r="B302" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C302">
         <v>2560</v>
@@ -9668,12 +9668,12 @@
         <v>1500</v>
       </c>
       <c r="F302" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="303" spans="2:6">
       <c r="B303" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C303">
         <v>2560</v>
@@ -9685,12 +9685,12 @@
         <v>750</v>
       </c>
       <c r="F303" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="304" spans="2:6">
       <c r="B304" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C304">
         <v>2560</v>
@@ -9702,12 +9702,12 @@
         <v>375</v>
       </c>
       <c r="F304" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="305" spans="2:6">
       <c r="B305" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C305">
         <v>2560</v>
@@ -9719,12 +9719,12 @@
         <v>187</v>
       </c>
       <c r="F305" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="306" spans="2:6">
       <c r="B306" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C306">
         <v>512</v>
@@ -9736,12 +9736,12 @@
         <v>1</v>
       </c>
       <c r="F306" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="307" spans="2:6">
       <c r="B307" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C307">
         <v>512</v>
@@ -9753,12 +9753,12 @@
         <v>1</v>
       </c>
       <c r="F307" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="308" spans="2:6">
       <c r="B308" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C308">
         <v>512</v>
@@ -9770,12 +9770,12 @@
         <v>1</v>
       </c>
       <c r="F308" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="309" spans="2:6">
       <c r="B309" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C309">
         <v>1024</v>
@@ -9787,12 +9787,12 @@
         <v>1500</v>
       </c>
       <c r="F309" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="310" spans="2:6">
       <c r="B310" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C310">
         <v>1024</v>
@@ -9804,12 +9804,12 @@
         <v>1500</v>
       </c>
       <c r="F310" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="311" spans="2:6">
       <c r="B311" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C311">
         <v>1024</v>
@@ -9821,7 +9821,7 @@
         <v>1500</v>
       </c>
       <c r="F311" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Keep width first for all convolution kernels in spreadsheets
</commit_message>
<xml_diff>
--- a/DeepBenchKernels_inference.xlsx
+++ b/DeepBenchKernels_inference.xlsx
@@ -248,8 +248,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="303">
+  <cellStyleXfs count="321">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -558,7 +576,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="303">
+  <cellStyles count="321">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -710,6 +728,15 @@
     <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -861,6 +888,15 @@
     <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="319" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1205,6 +1241,7 @@
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
     <col min="7" max="7" width="18.1640625" customWidth="1"/>
     <col min="8" max="8" width="19.83203125" customWidth="1"/>
@@ -4026,22 +4063,22 @@
         <v>36</v>
       </c>
       <c r="H117" t="s">
+        <v>56</v>
+      </c>
+      <c r="I117" t="s">
         <v>55</v>
       </c>
-      <c r="I117" t="s">
-        <v>56</v>
-      </c>
       <c r="J117" t="s">
+        <v>21</v>
+      </c>
+      <c r="K117" t="s">
         <v>20</v>
       </c>
-      <c r="K117" t="s">
-        <v>21</v>
-      </c>
       <c r="L117" t="s">
+        <v>23</v>
+      </c>
+      <c r="M117" t="s">
         <v>22</v>
-      </c>
-      <c r="M117" t="s">
-        <v>23</v>
       </c>
       <c r="N117" t="s">
         <v>43</v>
@@ -4076,10 +4113,10 @@
         <v>32</v>
       </c>
       <c r="H118">
+        <v>20</v>
+      </c>
+      <c r="I118">
         <v>5</v>
-      </c>
-      <c r="I118">
-        <v>20</v>
       </c>
       <c r="J118">
         <v>0</v>
@@ -4117,10 +4154,10 @@
         <v>32</v>
       </c>
       <c r="H119">
+        <v>20</v>
+      </c>
+      <c r="I119">
         <v>5</v>
-      </c>
-      <c r="I119">
-        <v>20</v>
       </c>
       <c r="J119">
         <v>0</v>
@@ -4158,10 +4195,10 @@
         <v>32</v>
       </c>
       <c r="H120">
+        <v>20</v>
+      </c>
+      <c r="I120">
         <v>5</v>
-      </c>
-      <c r="I120">
-        <v>20</v>
       </c>
       <c r="J120">
         <v>0</v>
@@ -4199,10 +4236,10 @@
         <v>32</v>
       </c>
       <c r="H121">
+        <v>10</v>
+      </c>
+      <c r="I121">
         <v>5</v>
-      </c>
-      <c r="I121">
-        <v>10</v>
       </c>
       <c r="J121">
         <v>0</v>
@@ -4240,10 +4277,10 @@
         <v>32</v>
       </c>
       <c r="H122">
+        <v>10</v>
+      </c>
+      <c r="I122">
         <v>5</v>
-      </c>
-      <c r="I122">
-        <v>10</v>
       </c>
       <c r="J122">
         <v>0</v>
@@ -4281,10 +4318,10 @@
         <v>32</v>
       </c>
       <c r="H123">
+        <v>10</v>
+      </c>
+      <c r="I123">
         <v>5</v>
-      </c>
-      <c r="I123">
-        <v>10</v>
       </c>
       <c r="J123">
         <v>0</v>
@@ -5772,11 +5809,11 @@
       <c r="K159">
         <v>8</v>
       </c>
-      <c r="L159" s="2">
-        <v>2</v>
-      </c>
-      <c r="M159">
+      <c r="L159">
         <v>8</v>
+      </c>
+      <c r="M159" s="2">
+        <v>2</v>
       </c>
       <c r="N159" t="s">
         <v>46</v>

</xml_diff>